<commit_message>
bash para deletar logs adicionado funcao custo agora sendo localizada pela sua posicao no campo objetos estao sendo limpos apos o programa ser reiniciado
</commit_message>
<xml_diff>
--- a/ProjetoFinalQT/ProjetoFinal/ganhos.xlsx
+++ b/ProjetoFinalQT/ProjetoFinal/ganhos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,14 +9,81 @@
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+  <si>
+    <t>__roboData__saved_ESC1_orientacao_otimo90</t>
+  </si>
+  <si>
+    <t>kp</t>
+  </si>
+  <si>
+    <t>kd</t>
+  </si>
+  <si>
+    <t>ki</t>
+  </si>
+  <si>
+    <t>senoide</t>
+  </si>
+  <si>
+    <t>(30 * M_PI / 180.0)*sin(2 * M_PI * 1 * t)</t>
+  </si>
+  <si>
+    <t>omegaH LOWPASS</t>
+  </si>
+  <si>
+    <t>omegaH LOWPASS2</t>
+  </si>
+  <si>
+    <t>__roboData__saved_ESC1_orientacao_otimo90_perturbacaoJacoud</t>
+  </si>
+  <si>
+    <t>roboData_saved_identificacao_pid55</t>
+  </si>
+  <si>
+    <t>(30 * M_PI / 180)+(30 * M_PI / 180.0)*sin(2 * M_PI * 1 * t)</t>
+  </si>
+  <si>
+    <t>Jitter func</t>
+  </si>
+  <si>
+    <t>(0.5*sin(2 * 3.141592 * 20 * t))</t>
+  </si>
+  <si>
+    <t>gain robot</t>
+  </si>
+  <si>
+    <t>dead zone</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>_signalStream_saved_identificacao_jitter (tanto no robot qto na simulacao)</t>
+  </si>
+  <si>
+    <t>_signalStream_saved_identificacao_jitter (apenas no robot)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -44,21 +111,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -96,9 +178,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +215,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -168,7 +250,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -341,13 +423,209 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="69.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>55</v>
+      </c>
+      <c r="E2" s="2">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.01</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
+        <v>0.5</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="2">
+        <v>26</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>